<commit_message>
added tests for greedy algorithm
</commit_message>
<xml_diff>
--- a/test_back/IntegrationTestsBackend/TestCasesShapesCatalinAnton.xlsx
+++ b/test_back/IntegrationTestsBackend/TestCasesShapesCatalinAnton.xlsx
@@ -17,7 +17,6 @@
     <sheet name="Questions" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="71">
   <si>
     <t>Preconditions</t>
   </si>
@@ -36,9 +35,6 @@
   </si>
   <si>
     <t>Expected Results</t>
-  </si>
-  <si>
-    <t>Actual results</t>
   </si>
   <si>
     <t>Remarks</t>
@@ -433,9 +429,6 @@
       </rPr>
       <t>"</t>
     </r>
-  </si>
-  <si>
-    <t>still produces a file jsonoutput.json</t>
   </si>
   <si>
     <t>Give figura13.json as input, to make a graph of pieces for it. It is a tube made of rectangles</t>
@@ -617,6 +610,67 @@
   </si>
   <si>
     <t>Catalin Anton</t>
+  </si>
+  <si>
+    <t>on greedy, it works</t>
+  </si>
+  <si>
+    <t>failed on greedy, doesn’t stop</t>
+  </si>
+  <si>
+    <t>idem</t>
+  </si>
+  <si>
+    <t>Greedy Result</t>
+  </si>
+  <si>
+    <t>Standard Result</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TEST PASSED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">              </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>TEST FAILED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                  (it doesn't stop)</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1074,10 +1128,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:J13"/>
+  <dimension ref="A2:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1089,30 +1143,30 @@
     <col min="5" max="5" width="22.28515625" customWidth="1"/>
     <col min="6" max="6" width="32" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="9" max="9" width="23.140625" customWidth="1"/>
+    <col min="8" max="9" width="18.5703125" customWidth="1"/>
+    <col min="10" max="10" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>0</v>
@@ -1124,286 +1178,340 @@
         <v>2</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="J3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="I3" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
     </row>
-    <row r="4" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="E4" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>20</v>
-      </c>
       <c r="H4" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>2</v>
       </c>
       <c r="B5" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="D5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="F5" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H5" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H5" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="I5" t="s">
-        <v>33</v>
+      <c r="I5" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="K5" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="I6" s="15" t="s">
+        <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>39</v>
+      <c r="I7" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="K7" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>5</v>
       </c>
       <c r="B8" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>43</v>
-      </c>
       <c r="F8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="K8" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>46</v>
+      <c r="I9" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="K9" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="I10" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="J10" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C10" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>49</v>
+      <c r="K10" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>8</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K11" t="s">
+        <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="300" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="300" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>9</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>59</v>
-      </c>
       <c r="E12" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>56</v>
+        <v>44</v>
+      </c>
+      <c r="I12" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="K12" s="6" t="s">
+        <v>66</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="165" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="165" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>10</v>
       </c>
       <c r="B13" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>63</v>
-      </c>
       <c r="F13" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>60</v>
+        <v>20</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1433,36 +1541,36 @@
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="I5" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>